<commit_message>
modify example data (simplified parameters)
</commit_message>
<xml_diff>
--- a/inst/extdata/liste_ind_coll_ex.xlsx
+++ b/inst/extdata/liste_ind_coll_ex.xlsx
@@ -17,12 +17,12 @@
     <sheet name="Print_parameters_ex2" sheetId="3" r:id="rId3"/>
     <sheet name="Table_data" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="57">
   <si>
     <t>name</t>
   </si>
@@ -66,18 +66,9 @@
     <t>order of print on the label (max 4; labels are limited to 4 lines)</t>
   </si>
   <si>
-    <t>print_field_name</t>
-  </si>
-  <si>
-    <t>Shoudl a field name (often abbreviation) be printed ? (1 = YES)</t>
-  </si>
-  <si>
     <t>field_name_to_print</t>
   </si>
   <si>
-    <t>If print_field_name = 1, what field name (prefix abbre) should be printed (note that some characters such as “_” creates bugs when compiling to pdf)</t>
-  </si>
-  <si>
     <t>print_opt_it</t>
   </si>
   <si>
@@ -196,6 +187,13 @@
   </si>
   <si>
     <t>pipiens</t>
+  </si>
+  <si>
+    <t>prefix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prefix (abbreviation) to be printed in front of the data, if any.
+</t>
   </si>
 </sst>
 </file>
@@ -388,7 +386,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -396,6 +394,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="19">
     <cellStyle name="Accent" xfId="1"/>
@@ -694,9 +693,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
@@ -765,76 +766,65 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
+        <v>4</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:3">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>7</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -848,18 +838,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="4" width="12.140625" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="11" width="12.140625" customWidth="1"/>
+    <col min="1" max="10" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -873,30 +863,27 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -907,13 +894,13 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -924,13 +911,13 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -942,25 +929,25 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -971,19 +958,16 @@
       <c r="D7">
         <v>1</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="E7" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -994,19 +978,16 @@
       <c r="D8">
         <v>2</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>36</v>
-      </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1017,13 +998,13 @@
       <c r="D9">
         <v>4</v>
       </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1034,13 +1015,13 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1051,16 +1032,16 @@
       <c r="D11">
         <v>2</v>
       </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
       <c r="G11">
         <v>1</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1071,24 +1052,24 @@
       <c r="D12">
         <v>3</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1099,13 +1080,10 @@
       <c r="D14">
         <v>3</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14" t="s">
-        <v>43</v>
-      </c>
-      <c r="J14">
+      <c r="E14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14">
         <v>1</v>
       </c>
     </row>
@@ -1120,16 +1098,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="11" width="12.140625" customWidth="1"/>
+    <col min="1" max="10" width="12.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1143,30 +1123,27 @@
         <v>12</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J1" t="s">
-        <v>24</v>
-      </c>
-      <c r="K1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1177,13 +1154,13 @@
       <c r="D2">
         <v>1</v>
       </c>
-      <c r="I2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="H2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1194,13 +1171,13 @@
       <c r="D3">
         <v>2</v>
       </c>
-      <c r="I3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1211,13 +1188,13 @@
       <c r="D4">
         <v>3</v>
       </c>
-      <c r="I4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -1229,9 +1206,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:10">
       <c r="A6" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -1243,9 +1220,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:11">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -1256,19 +1233,16 @@
       <c r="D7">
         <v>5</v>
       </c>
-      <c r="E7">
-        <v>1</v>
-      </c>
-      <c r="F7" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="E7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -1279,16 +1253,13 @@
       <c r="D8">
         <v>6</v>
       </c>
-      <c r="E8">
-        <v>1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="E8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>1</v>
@@ -1299,16 +1270,16 @@
       <c r="D9">
         <v>4</v>
       </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1319,13 +1290,13 @@
       <c r="D10">
         <v>1</v>
       </c>
-      <c r="G10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1336,16 +1307,16 @@
       <c r="D11">
         <v>2</v>
       </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
       <c r="G11">
         <v>1</v>
       </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11">
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1356,21 +1327,21 @@
       <c r="D12">
         <v>3</v>
       </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:11">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -1402,78 +1373,78 @@
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" t="s">
         <v>39</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="M1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:13">
       <c r="A2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="F2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -1484,37 +1455,37 @@
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="F3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -1525,37 +1496,37 @@
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="K4" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -1566,37 +1537,37 @@
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="F5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="J5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="1" t="s">
+      <c r="K5" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -1607,37 +1578,37 @@
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="F6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L6">
         <v>2</v>
@@ -1648,35 +1619,35 @@
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="F7" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="L7">
         <v>2</v>
@@ -1687,37 +1658,37 @@
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="F8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="I8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="K8" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L8">
         <v>2</v>
@@ -1728,37 +1699,37 @@
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="F9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="I9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L9">
         <v>1</v>
@@ -1769,37 +1740,37 @@
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="E10" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="F10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="I10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="J10" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K10" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -1810,37 +1781,37 @@
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="E11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="2" t="s">
+      <c r="F11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="I11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -1851,37 +1822,37 @@
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="E12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="2" t="s">
+      <c r="F12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="I12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L12">
         <v>1</v>
@@ -1892,37 +1863,37 @@
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="E13" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="2" t="s">
+      <c r="F13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="I13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L13">
         <v>1</v>
@@ -1933,37 +1904,37 @@
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="E14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="2" t="s">
+      <c r="F14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H14" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="I14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K14" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L14">
         <v>1</v>
@@ -1974,37 +1945,37 @@
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="E15" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="2" t="s">
+      <c r="F15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="I15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L15">
         <v>1</v>
@@ -2015,37 +1986,37 @@
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="E16" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="2" t="s">
+      <c r="F16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="I16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L16">
         <v>1</v>
@@ -2056,37 +2027,37 @@
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="E17" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="2" t="s">
+      <c r="F17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="I17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L17">
         <v>1</v>
@@ -2097,37 +2068,37 @@
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="E18" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="2" t="s">
+      <c r="F18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="I18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L18">
         <v>1</v>
@@ -2138,37 +2109,37 @@
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="E19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="2" t="s">
+      <c r="F19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="I19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L19">
         <v>1</v>
@@ -2179,37 +2150,37 @@
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="E20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="F20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="I20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L20">
         <v>1</v>
@@ -2220,37 +2191,37 @@
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="E21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="2" t="s">
+      <c r="F21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H21" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="I21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L21">
         <v>1</v>
@@ -2261,37 +2232,37 @@
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="E22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D22" s="2" t="s">
+      <c r="F22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H22" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="I22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L22">
         <v>1</v>
@@ -2302,37 +2273,37 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="E23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="2" t="s">
+      <c r="F23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="I23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L23">
         <v>1</v>
@@ -2343,37 +2314,37 @@
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="E24" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D24" s="2" t="s">
+      <c r="F24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H24" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="I24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L24">
         <v>1</v>
@@ -2384,37 +2355,37 @@
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="E25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="2" t="s">
+      <c r="F25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H25" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="I25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G25" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="H25" s="1" t="s">
+      <c r="K25" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>54</v>
       </c>
       <c r="L25">
         <v>1</v>

</xml_diff>